<commit_message>
Add tests for population variables
</commit_message>
<xml_diff>
--- a/output3.xlsx
+++ b/output3.xlsx
@@ -1203,6 +1203,12 @@
       <c r="AC4">
         <v>368.7791</v>
       </c>
+      <c r="AD4">
+        <v>391.2626588110001</v>
+      </c>
+      <c r="AE4">
+        <v>412.5551113083447</v>
+      </c>
     </row>
     <row r="5" spans="1:31">
       <c r="A5" t="s">
@@ -1292,6 +1298,12 @@
       <c r="AC5">
         <v>371.8565</v>
       </c>
+      <c r="AD5">
+        <v>394.2290174485</v>
+      </c>
+      <c r="AE5">
+        <v>416.7214275212921</v>
+      </c>
     </row>
     <row r="6" spans="1:31">
       <c r="A6" t="s">
@@ -1921,6 +1933,12 @@
       <c r="AC12">
         <v>2.012799999999999</v>
       </c>
+      <c r="AD12">
+        <v>1.862144777000012</v>
+      </c>
+      <c r="AE12">
+        <v>3.139585926351273</v>
+      </c>
     </row>
     <row r="13" spans="1:31">
       <c r="A13" t="s">
@@ -2010,6 +2028,12 @@
       <c r="AC13">
         <v>3.077399999999955</v>
       </c>
+      <c r="AD13">
+        <v>2.96635863749998</v>
+      </c>
+      <c r="AE13">
+        <v>4.166316212947322</v>
+      </c>
     </row>
     <row r="14" spans="1:31">
       <c r="A14" t="s">
@@ -2265,8 +2289,14 @@
       <c r="AC16">
         <v>92.0646</v>
       </c>
+      <c r="AD16">
+        <v>96.00819525389991</v>
+      </c>
+      <c r="AE16">
+        <v>99.4222724380695</v>
+      </c>
     </row>
-    <row r="17" spans="1:29">
+    <row r="17" spans="1:31">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -2354,8 +2384,14 @@
       <c r="AC17">
         <v>21.9499</v>
       </c>
+      <c r="AD17">
+        <v>23.11901260229315</v>
+      </c>
+      <c r="AE17">
+        <v>24.24488483060908</v>
+      </c>
     </row>
-    <row r="18" spans="1:29">
+    <row r="18" spans="1:31">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -2444,7 +2480,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="19" spans="1:29">
+    <row r="19" spans="1:31">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -2532,8 +2568,14 @@
       <c r="AC19" t="s">
         <v>151</v>
       </c>
+      <c r="AD19">
+        <v>443.2633733300499</v>
+      </c>
+      <c r="AE19">
+        <v>457.6293185330783</v>
+      </c>
     </row>
-    <row r="20" spans="1:29">
+    <row r="20" spans="1:31">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -2622,7 +2664,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="21" spans="1:29">
+    <row r="21" spans="1:31">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -2710,8 +2752,14 @@
       <c r="AC21" t="s">
         <v>152</v>
       </c>
+      <c r="AD21">
+        <v>449.15827333005</v>
+      </c>
+      <c r="AE21">
+        <v>463.5242185330783</v>
+      </c>
     </row>
-    <row r="22" spans="1:29">
+    <row r="22" spans="1:31">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -2800,7 +2848,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="23" spans="1:29">
+    <row r="23" spans="1:31">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -2888,8 +2936,14 @@
       <c r="AC23" t="s">
         <v>153</v>
       </c>
+      <c r="AD23">
+        <v>843.38729077855</v>
+      </c>
+      <c r="AE23">
+        <v>880.2456460543705</v>
+      </c>
     </row>
-    <row r="24" spans="1:29">
+    <row r="24" spans="1:31">
       <c r="A24" t="s">
         <v>4</v>
       </c>
@@ -2978,7 +3032,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="25" spans="1:29">
+    <row r="25" spans="1:31">
       <c r="A25" t="s">
         <v>4</v>
       </c>
@@ -3065,6 +3119,12 @@
       </c>
       <c r="AC25" t="s">
         <v>154</v>
+      </c>
+      <c r="AD25">
+        <v>112.7745918852599</v>
+      </c>
+      <c r="AE25">
+        <v>117.015989963076</v>
       </c>
     </row>
   </sheetData>

</xml_diff>